<commit_message>
finished timing stuff, working on saving
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -965,7 +965,9 @@
       <c r="C15" s="20">
         <v>16</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="20">
+        <v>7</v>
+      </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -981,7 +983,7 @@
       <c r="Q15" s="20"/>
       <c r="R15" s="20">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished saving for examinee
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -966,9 +966,11 @@
         <v>16</v>
       </c>
       <c r="D15" s="20">
+        <v>10</v>
+      </c>
+      <c r="E15" s="20">
         <v>7</v>
       </c>
-      <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
@@ -983,7 +985,7 @@
       <c r="Q15" s="20"/>
       <c r="R15" s="20">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished course manager tab ui
Work on updating course information
CourseManager class neraly complete
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -905,7 +905,9 @@
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="20">
+        <v>5</v>
+      </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -919,7 +921,7 @@
       <c r="Q13" s="20"/>
       <c r="R13" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1038,7 +1040,9 @@
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="20">
+        <v>5</v>
+      </c>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -1051,7 +1055,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Work on the course manager
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1043,9 @@
       <c r="G17" s="20">
         <v>5</v>
       </c>
-      <c r="H17" s="20"/>
+      <c r="H17" s="20">
+        <v>10</v>
+      </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
@@ -1055,7 +1057,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added import students function
Fixed bug with semester
Added edited flags to changing year and semester
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -1044,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="20">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -1057,7 +1057,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Prompt to apply course changes on closing
Fixed bug when saving courses
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -1044,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="20">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
@@ -1057,7 +1057,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
PDF completed using iTextSharp
UI for publishing mostly completed
Work begun on publishing code
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -910,7 +910,9 @@
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="I13" s="20">
+        <v>2</v>
+      </c>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -921,7 +923,7 @@
       <c r="Q13" s="20"/>
       <c r="R13" s="20">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1046,7 +1048,9 @@
       <c r="H17" s="20">
         <v>14</v>
       </c>
-      <c r="I17" s="20"/>
+      <c r="I17" s="20">
+        <v>13</v>
+      </c>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
@@ -1057,7 +1061,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
More work on publishing
</commit_message>
<xml_diff>
--- a/Time plan Sem2.xlsx
+++ b/Time plan Sem2.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A2:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1051,9 @@
       <c r="I17" s="20">
         <v>13</v>
       </c>
-      <c r="J17" s="20"/>
+      <c r="J17" s="20">
+        <v>12</v>
+      </c>
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
       <c r="M17" s="20"/>
@@ -1061,7 +1063,7 @@
       <c r="Q17" s="20"/>
       <c r="R17" s="20">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>